<commit_message>
More revisions to damped hip joint
Continued modifications to hip/femur pieces for new dampers and springs
</commit_message>
<xml_diff>
--- a/CAD_Mechanical/AARL_QR-Quadruped/AARL_QR_FR-Frame/InProgress/Haonan/AARL_QR_FR_LE_BI_BL-Back_Left_new/New Spring Dimensions.xlsx
+++ b/CAD_Mechanical/AARL_QR-Quadruped/AARL_QR_FR-Frame/InProgress/Haonan/AARL_QR_FR_LE_BI_BL-Back_Left_new/New Spring Dimensions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Quadruped_Robot\CAD_Mechanical\AARL_QR-Quadruped\AARL_QR_FR-Frame\InProgress\Haonan\AARL_QR_FR_LE_BI_BL-Back_Left_new\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tsclient\C\GitHub\Quadruped_Robot\CAD_Mechanical\AARL_QR-Quadruped\AARL_QR_FR-Frame\InProgress\Haonan\AARL_QR_FR_LE_BI_BL-Back_Left_new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{574F90CB-3C9A-4E63-8145-47AC0156D2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA56EB90-5465-464C-A6B4-04B8A3FF12E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{AA96BDC6-3A9B-4C76-9D78-C4C8DF3570E9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t>N-m/rad</t>
   </si>
@@ -98,6 +98,15 @@
   <si>
     <t>wire diameter
 (mm)                                                              (in)</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>first iteration of calculations - wanted higher number of coils but ended up being too wide</t>
+  </si>
+  <si>
+    <t>second iteration of calculations - fewer coils</t>
   </si>
 </sst>
 </file>
@@ -154,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -167,6 +176,16 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -175,13 +194,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,12 +523,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -590,10 +603,10 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="7"/>
+      <c r="B10" s="13"/>
       <c r="G10" t="s">
         <v>4</v>
       </c>
@@ -636,8 +649,8 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -652,27 +665,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CCADA16-F37A-4E24-B4B4-CAC4D5F5F2A3}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G21"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="3" max="7" width="29.85546875" customWidth="1"/>
+    <col min="9" max="9" width="73.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="9" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="9"/>
+      <c r="D1" s="15"/>
       <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
@@ -682,8 +696,11 @@
       <c r="G1" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I1" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>40</v>
       </c>
@@ -711,7 +728,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>19</v>
       </c>
@@ -738,7 +755,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>40</v>
       </c>
@@ -765,7 +782,7 @@
         <v>27.343989054843124</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>19</v>
       </c>
@@ -792,7 +809,7 @@
         <v>27.645566906995271</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <f>(($B$21*1000000000)*(C8/1000)^4)/(64*(F8/1000)*E8)</f>
         <v>39.648200098975394</v>
@@ -804,23 +821,26 @@
         <f>CONVERT(D8,"in","mm")</f>
         <v>7.1437499999999998</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="9">
         <f>9/32</f>
         <v>0.28125</v>
       </c>
       <c r="E8">
         <v>6</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="11">
         <f>G8+C8</f>
         <v>34.793749999999996</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="10">
         <f>27.65</f>
         <v>27.65</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <f>(($B$21*1000000000)*(C9/1000)^4)/(64*(F9/1000)*E9)</f>
         <v>18.997522683320884</v>
@@ -832,30 +852,139 @@
         <f>CONVERT(D9,"in","mm")</f>
         <v>6.35</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="9">
         <f>1/4</f>
         <v>0.25</v>
       </c>
       <c r="E9">
         <v>8</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="11">
         <f>G9+C9</f>
         <v>34</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="10">
         <f>27.65</f>
         <v>27.65</v>
       </c>
     </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <f>CONVERT(D11,"in","mm")</f>
+        <v>6.35</v>
+      </c>
+      <c r="D11" s="6">
+        <f>8/32</f>
+        <v>0.25</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" s="5">
+        <f>((($B$21*1000000000)*(C11/1000)^4)/(64*A11*E11))*1000</f>
+        <v>32.295788561645509</v>
+      </c>
+      <c r="G11" s="1">
+        <f>F11-C11</f>
+        <v>25.945788561645507</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <f>CONVERT(D12,"in","mm")</f>
+        <v>5.5562500000000004</v>
+      </c>
+      <c r="D12" s="16">
+        <f>7/32</f>
+        <v>0.21875</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12" s="5">
+        <f>((($B$21*1000000000)*(C12/1000)^4)/(64*A12*E12))*1000</f>
+        <v>31.884123493631115</v>
+      </c>
+      <c r="G12" s="1">
+        <f>F12-C12</f>
+        <v>26.327873493631117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <f>(($B$21*1000000000)*(C14/1000)^4)/(64*(F14/1000)*E14)</f>
+        <v>39.74866284510216</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <f>CONVERT(D14,"in","mm")</f>
+        <v>6.35</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14" s="11">
+        <f>G14+C14</f>
+        <v>32.5</v>
+      </c>
+      <c r="G14" s="10">
+        <v>26.15</v>
+      </c>
+      <c r="I14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <f>(($B$21*1000000000)*(C15/1000)^4)/(64*(F15/1000)*E15)</f>
+        <v>19.106590857606662</v>
+      </c>
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <f>CONVERT(D15,"in","mm")</f>
+        <v>5.5562500000000004</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0.21875</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15" s="11">
+        <f>G15+C15</f>
+        <v>31.706249999999997</v>
+      </c>
+      <c r="G15" s="10">
+        <v>26.15</v>
+      </c>
+    </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="8">
         <v>203.4</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="8" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Damped Hind Leg Assembly Changes
Continued modifications to pelvis and femur to accommodate new springs and dampers
</commit_message>
<xml_diff>
--- a/CAD_Mechanical/AARL_QR-Quadruped/AARL_QR_FR-Frame/InProgress/Haonan/AARL_QR_FR_LE_BI_BL-Back_Left_new/New Spring Dimensions.xlsx
+++ b/CAD_Mechanical/AARL_QR-Quadruped/AARL_QR_FR-Frame/InProgress/Haonan/AARL_QR_FR_LE_BI_BL-Back_Left_new/New Spring Dimensions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tsclient\C\GitHub\Quadruped_Robot\CAD_Mechanical\AARL_QR-Quadruped\AARL_QR_FR-Frame\InProgress\Haonan\AARL_QR_FR_LE_BI_BL-Back_Left_new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA56EB90-5465-464C-A6B4-04B8A3FF12E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFFE9F7-B63D-474E-A246-28FF77446984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{AA96BDC6-3A9B-4C76-9D78-C4C8DF3570E9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
   <si>
     <t>N-m/rad</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>second iteration of calculations - fewer coils</t>
+  </si>
+  <si>
+    <t xml:space="preserve">third iteration of calculations - add an eighth of a coil </t>
   </si>
 </sst>
 </file>
@@ -185,6 +188,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -194,7 +198,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,12 +526,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -603,10 +606,10 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="13"/>
+      <c r="B10" s="14"/>
       <c r="G10" t="s">
         <v>4</v>
       </c>
@@ -649,8 +652,8 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -665,10 +668,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CCADA16-F37A-4E24-B4B4-CAC4D5F5F2A3}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,14 +682,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="15"/>
+      <c r="D1" s="16"/>
       <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
@@ -716,7 +719,7 @@
         <v>0.25</v>
       </c>
       <c r="E2" s="5">
-        <f>(($B$21*1000000000)*(C2/1000)^4)/(64*(F2/1000)*A2)</f>
+        <f>(($B$26*1000000000)*(C2/1000)^4)/(64*(F2/1000)*A2)</f>
         <v>4.0687607636718743</v>
       </c>
       <c r="F2">
@@ -743,7 +746,7 @@
         <v>0.25</v>
       </c>
       <c r="E3" s="5">
-        <f>(($B$21*1000000000)*(C3/1000)^4)/(64*(F3/1000)*A3)</f>
+        <f>(($B$26*1000000000)*(C3/1000)^4)/(64*(F3/1000)*A3)</f>
         <v>8.5658121340460518</v>
       </c>
       <c r="F3">
@@ -774,7 +777,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="5">
-        <f>((($B$21*1000000000)*(C5/1000)^4)/(64*A5*E5))*1000</f>
+        <f>((($B$26*1000000000)*(C5/1000)^4)/(64*A5*E5))*1000</f>
         <v>34.487739054843125</v>
       </c>
       <c r="G5" s="1">
@@ -801,7 +804,7 @@
         <v>8</v>
       </c>
       <c r="F6" s="5">
-        <f>((($B$21*1000000000)*(C6/1000)^4)/(64*A6*E6))*1000</f>
+        <f>((($B$26*1000000000)*(C6/1000)^4)/(64*A6*E6))*1000</f>
         <v>33.995566906995272</v>
       </c>
       <c r="G6" s="1">
@@ -811,7 +814,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <f>(($B$21*1000000000)*(C8/1000)^4)/(64*(F8/1000)*E8)</f>
+        <f>(($B$26*1000000000)*(C8/1000)^4)/(64*(F8/1000)*E8)</f>
         <v>39.648200098975394</v>
       </c>
       <c r="B8" t="s">
@@ -842,7 +845,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <f>(($B$21*1000000000)*(C9/1000)^4)/(64*(F9/1000)*E9)</f>
+        <f>(($B$26*1000000000)*(C9/1000)^4)/(64*(F9/1000)*E9)</f>
         <v>18.997522683320884</v>
       </c>
       <c r="B9" t="s">
@@ -887,7 +890,7 @@
         <v>4</v>
       </c>
       <c r="F11" s="5">
-        <f>((($B$21*1000000000)*(C11/1000)^4)/(64*A11*E11))*1000</f>
+        <f>((($B$26*1000000000)*(C11/1000)^4)/(64*A11*E11))*1000</f>
         <v>32.295788561645509</v>
       </c>
       <c r="G11" s="1">
@@ -906,7 +909,7 @@
         <f>CONVERT(D12,"in","mm")</f>
         <v>5.5562500000000004</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="13">
         <f>7/32</f>
         <v>0.21875</v>
       </c>
@@ -914,7 +917,7 @@
         <v>5</v>
       </c>
       <c r="F12" s="5">
-        <f>((($B$21*1000000000)*(C12/1000)^4)/(64*A12*E12))*1000</f>
+        <f>((($B$26*1000000000)*(C12/1000)^4)/(64*A12*E12))*1000</f>
         <v>31.884123493631115</v>
       </c>
       <c r="G12" s="1">
@@ -924,7 +927,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <f>(($B$21*1000000000)*(C14/1000)^4)/(64*(F14/1000)*E14)</f>
+        <f>(($B$26*1000000000)*(C14/1000)^4)/(64*(F14/1000)*E14)</f>
         <v>39.74866284510216</v>
       </c>
       <c r="B14" t="s">
@@ -953,7 +956,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <f>(($B$21*1000000000)*(C15/1000)^4)/(64*(F15/1000)*E15)</f>
+        <f>(($B$26*1000000000)*(C15/1000)^4)/(64*(F15/1000)*E15)</f>
         <v>19.106590857606662</v>
       </c>
       <c r="B15" t="s">
@@ -977,14 +980,123 @@
         <v>26.15</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>40</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <f>CONVERT(D17,"in","mm")</f>
+        <v>6.35</v>
+      </c>
+      <c r="D17" s="6">
+        <f>8/32</f>
+        <v>0.25</v>
+      </c>
+      <c r="E17">
+        <v>4.125</v>
+      </c>
+      <c r="F17" s="5">
+        <f>((($B$26*1000000000)*(C17/1000)^4)/(64*A17*E17))*1000</f>
+        <v>31.317128302201702</v>
+      </c>
+      <c r="G17" s="1">
+        <f>F17-C17</f>
+        <v>24.967128302201701</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <f>CONVERT(D18,"in","mm")</f>
+        <v>5.5562500000000004</v>
+      </c>
+      <c r="D18" s="13">
+        <f>7/32</f>
+        <v>0.21875</v>
+      </c>
+      <c r="E18">
+        <v>5.125</v>
+      </c>
+      <c r="F18" s="5">
+        <f>((($B$26*1000000000)*(C18/1000)^4)/(64*A18*E18))*1000</f>
+        <v>31.106461945005965</v>
+      </c>
+      <c r="G18" s="1">
+        <f>F18-C18</f>
+        <v>25.550211945005962</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <f>(($B$26*1000000000)*(C20/1000)^4)/(64*(F20/1000)*E20)</f>
+        <v>39.641934559748982</v>
+      </c>
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <f>CONVERT(D20,"in","mm")</f>
+        <v>6.35</v>
+      </c>
+      <c r="D20" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="E20">
+        <v>4.125</v>
+      </c>
+      <c r="F20" s="11">
+        <f>G20+C20</f>
+        <v>31.6</v>
+      </c>
+      <c r="G20" s="10">
+        <v>25.25</v>
+      </c>
+      <c r="I20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <f>(($B$26*1000000000)*(C21/1000)^4)/(64*(F21/1000)*E21)</f>
+        <v>19.185158107692864</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <f>CONVERT(D21,"in","mm")</f>
+        <v>5.5562500000000004</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0.21875</v>
+      </c>
+      <c r="E21">
+        <v>5.125</v>
+      </c>
+      <c r="F21" s="11">
+        <f>G21+C21</f>
+        <v>30.806249999999999</v>
+      </c>
+      <c r="G21" s="10">
+        <v>25.25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B26" s="8">
         <v>203.4</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C26" s="8" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New hind leg subassemblies
Making new hind leg sub assemblies for center of mass calculation
</commit_message>
<xml_diff>
--- a/CAD_Mechanical/AARL_QR-Quadruped/AARL_QR_FR-Frame/InProgress/Haonan/AARL_QR_FR_LE_BI_BL-Back_Left_new/New Spring Dimensions.xlsx
+++ b/CAD_Mechanical/AARL_QR-Quadruped/AARL_QR_FR-Frame/InProgress/Haonan/AARL_QR_FR_LE_BI_BL-Back_Left_new/New Spring Dimensions.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Haonan\Documents\GitHub\Quadruped_Robot\CAD_Mechanical\AARL_QR-Quadruped\AARL_QR_FR-Frame\InProgress\Haonan\AARL_QR_FR_LE_BI_BL-Back_Left_new\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tsclient\C\GitHub\Quadruped_Robot\CAD_Mechanical\AARL_QR-Quadruped\AARL_QR_FR-Frame\InProgress\Haonan\AARL_QR_FR_LE_BI_BL-Back_Left_new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E2C080-2000-43DA-ABB2-62B897173A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D933D46-FF3E-47C2-A089-63CDD0638FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-180" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{AA96BDC6-3A9B-4C76-9D78-C4C8DF3570E9}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{AA96BDC6-3A9B-4C76-9D78-C4C8DF3570E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="56">
   <si>
     <t>N-m/rad</t>
   </si>
@@ -113,6 +114,99 @@
   </si>
   <si>
     <t>22.7mm mandrel OD for springback</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Mass (g)</t>
+  </si>
+  <si>
+    <t>BL_012v5</t>
+  </si>
+  <si>
+    <t>medium nut</t>
+  </si>
+  <si>
+    <t>BL_002.rat</t>
+  </si>
+  <si>
+    <t>post and screw</t>
+  </si>
+  <si>
+    <t>BL_003v3</t>
+  </si>
+  <si>
+    <t>BO_025v6</t>
+  </si>
+  <si>
+    <t>6597K8</t>
+  </si>
+  <si>
+    <t>6597K19</t>
+  </si>
+  <si>
+    <t>6597K118</t>
+  </si>
+  <si>
+    <t>6597K119</t>
+  </si>
+  <si>
+    <t>BL_011j2</t>
+  </si>
+  <si>
+    <t>BL_004v4</t>
+  </si>
+  <si>
+    <t>BL_005.rat</t>
+  </si>
+  <si>
+    <t>BL_011j3</t>
+  </si>
+  <si>
+    <t>BL_006v2</t>
+  </si>
+  <si>
+    <t>BL_007v2</t>
+  </si>
+  <si>
+    <t>BL_008</t>
+  </si>
+  <si>
+    <t>BL_009</t>
+  </si>
+  <si>
+    <t>BL_010</t>
+  </si>
+  <si>
+    <t>large nut</t>
+  </si>
+  <si>
+    <t>nuts (m)</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>encoder + mount small</t>
+  </si>
+  <si>
+    <t>encoder + mount large</t>
+  </si>
+  <si>
+    <t>dshaft 119mm</t>
+  </si>
+  <si>
+    <t>dshaft 80mm</t>
+  </si>
+  <si>
+    <t>dshaft 52mm</t>
+  </si>
+  <si>
+    <t>4-40 SHS 1250</t>
+  </si>
+  <si>
+    <t>4-40 SHS 0500</t>
   </si>
 </sst>
 </file>
@@ -667,7 +761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CCADA16-F37A-4E24-B4B4-CAC4D5F5F2A3}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
@@ -1108,4 +1202,406 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF7B2F4C-D259-48ED-AC54-C1F95C4B8EE6}">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="27.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2">
+        <v>44</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <f>B2-C2*$B$25</f>
+        <v>43.2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>23</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D28" si="0">B3-C3*$B$25</f>
+        <v>21.4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4">
+        <v>39</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6">
+        <v>38</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7">
+        <v>35</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>33.4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>9.6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>7.6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14">
+        <v>105</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>102.6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15">
+        <v>1.7</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>1.7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17">
+        <v>79</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="E17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18">
+        <v>79</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19">
+        <v>21</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20">
+        <v>28</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21">
+        <v>29</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23">
+        <v>12</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25">
+        <f>4/10</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="2">
+        <f>4/6</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27">
+        <f>13/10</f>
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28">
+        <f>2/4</f>
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Damped hind leg calculation
subassemblies to find center of mass

start formatting data in excel to calculate experimental damping ratios
</commit_message>
<xml_diff>
--- a/CAD_Mechanical/AARL_QR-Quadruped/AARL_QR_FR-Frame/InProgress/Haonan/AARL_QR_FR_LE_BI_BL-Back_Left_new/New Spring Dimensions.xlsx
+++ b/CAD_Mechanical/AARL_QR-Quadruped/AARL_QR_FR-Frame/InProgress/Haonan/AARL_QR_FR_LE_BI_BL-Back_Left_new/New Spring Dimensions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tsclient\C\GitHub\Quadruped_Robot\CAD_Mechanical\AARL_QR-Quadruped\AARL_QR_FR-Frame\InProgress\Haonan\AARL_QR_FR_LE_BI_BL-Back_Left_new\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Quadruped_Robot\CAD_Mechanical\AARL_QR-Quadruped\AARL_QR_FR-Frame\InProgress\Haonan\AARL_QR_FR_LE_BI_BL-Back_Left_new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D933D46-FF3E-47C2-A089-63CDD0638FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B30FFF-7CD4-4E05-8F58-B1240B6B4C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{AA96BDC6-3A9B-4C76-9D78-C4C8DF3570E9}"/>
+    <workbookView xWindow="-28920" yWindow="-180" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{AA96BDC6-3A9B-4C76-9D78-C4C8DF3570E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
   <si>
     <t>N-m/rad</t>
   </si>
@@ -207,6 +207,24 @@
   </si>
   <si>
     <t>4-40 SHS 0500</t>
+  </si>
+  <si>
+    <t>limb 1</t>
+  </si>
+  <si>
+    <t>limb 2</t>
+  </si>
+  <si>
+    <t>limb 3</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>measured new leg properties</t>
   </si>
 </sst>
 </file>
@@ -1206,10 +1224,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF7B2F4C-D259-48ED-AC54-C1F95C4B8EE6}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1217,7 +1235,7 @@
     <col min="1" max="2" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -1228,7 +1246,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1246,7 +1264,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1257,14 +1275,14 @@
         <v>4</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D28" si="0">B3-C3*$B$25</f>
+        <f t="shared" ref="D3:D24" si="0">B3-C3*$B$25</f>
         <v>21.4</v>
       </c>
       <c r="E3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1279,7 +1297,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1291,7 +1309,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1305,8 +1323,14 @@
       <c r="E6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H6" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1323,8 +1347,17 @@
       <c r="E7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>59</v>
+      </c>
+      <c r="J7" t="s">
+        <v>60</v>
+      </c>
+      <c r="K7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -1335,8 +1368,20 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8">
+        <v>190.04</v>
+      </c>
+      <c r="J8">
+        <v>130.77000000000001</v>
+      </c>
+      <c r="K8">
+        <v>192.72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1350,8 +1395,20 @@
       <c r="E9" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9">
+        <v>267.99700000000001</v>
+      </c>
+      <c r="J9">
+        <v>171.35</v>
+      </c>
+      <c r="K9">
+        <v>166.26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1365,8 +1422,20 @@
       <c r="E10" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10">
+        <v>162.02000000000001</v>
+      </c>
+      <c r="J10">
+        <v>53.49</v>
+      </c>
+      <c r="K10">
+        <v>35.33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -1384,7 +1453,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1402,7 +1471,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -1417,7 +1486,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1435,7 +1504,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1450,7 +1519,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1602,6 +1671,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H6:K6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>